<commit_message>
Completed Data Entry form course, TODO Update README
</commit_message>
<xml_diff>
--- a/beginners-da-course-chandoo/beginner-DA-course.xlsx
+++ b/beginners-da-course-chandoo/beginner-DA-course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\microsoft-excel\beginners-da-course-chandoo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD8444C-EC90-41B0-8612-1DECD69DBFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9A9263-E5A2-49E5-A505-263AFEFDE95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{26D4546B-D2A1-4444-8EAF-A6228F96F0C1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{26D4546B-D2A1-4444-8EAF-A6228F96F0C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'3'!$E$8:$H$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$C$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">'6'!$N$6:$N$305</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'6'!$P$6:$P$305</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'6'!$P$6:$P$305</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'6'!$N$6:$N$305</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'6'!$P$6:$P$305</definedName>
     <definedName name="_xlcn.WorksheetConnection_beginnerDAcourse.xlsxdata1" hidden="1">data[]</definedName>
     <definedName name="Slicer_Geography">#N/A</definedName>
@@ -42,7 +42,7 @@
     <pivotCache cacheId="0" r:id="rId13"/>
     <pivotCache cacheId="1" r:id="rId14"/>
     <pivotCache cacheId="2" r:id="rId15"/>
-    <pivotCache cacheId="40" r:id="rId16"/>
+    <pivotCache cacheId="3" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -770,7 +770,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="27">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -830,6 +830,36 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.249977111117893"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -935,7 +965,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{EB3F2A35-CE4A-479B-A858-DB4065808036}">
-      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -3041,7 +3071,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3103,10 +3133,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5318,8 +5348,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>69274</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Geography 1">
@@ -5342,7 +5372,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -7975,7 +8005,7 @@
     <dataField name="Sum of Units" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="9">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -8118,6 +8148,121 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85974051-05D3-438C-8B5E-D54A5C41579E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D7:E20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0" measureFilter="1" sortType="descending">
+      <items count="11">
+        <item x="7"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="9"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="4"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="6" showAll="0"/>
+    <pivotField numFmtId="3" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Amount" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="0" type="count" evalOrder="-1" id="2" iMeasureFld="0">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <top10 top="0" val="1" filterVal="1"/>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{22CF0ACB-50C5-447D-AD72-66CFDCF8EA32}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
@@ -8217,121 +8362,6 @@
       <autoFilter ref="A1">
         <filterColumn colId="0">
           <top10 val="1" filterVal="1"/>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-  </filters>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85974051-05D3-438C-8B5E-D54A5C41579E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D7:E20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0" measureFilter="1" sortType="descending">
-      <items count="11">
-        <item x="7"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="9"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="4"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="6" showAll="0"/>
-    <pivotField numFmtId="3" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="1"/>
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="13">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Amount" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="1">
-    <filter fld="0" type="count" evalOrder="-1" id="2" iMeasureFld="0">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <top10 top="0" val="1" filterVal="1"/>
         </filterColumn>
       </autoFilter>
     </filter>
@@ -8507,7 +8537,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{30ED8A61-487A-4D76-913F-6A0FF0600330}" name="PivotTable4" cacheId="40" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{30ED8A61-487A-4D76-913F-6A0FF0600330}" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A8:E29" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -8830,25 +8860,25 @@
   <autoFilter ref="O11:P33" xr:uid="{6DAC1E92-D947-4232-891E-65555AD7A47E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1B8963D1-E60F-4400-A175-651A513B826F}" name="Product"/>
-    <tableColumn id="2" xr3:uid="{1798A7DA-FB9F-46D3-AA0A-B6BCA4A81AC3}" name="Cost per unit" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{1798A7DA-FB9F-46D3-AA0A-B6BCA4A81AC3}" name="Cost per unit" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1EA555D6-243D-4A1C-9B7C-CE41EE1BDD83}" name="data" displayName="data" ref="A1:G301" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1EA555D6-243D-4A1C-9B7C-CE41EE1BDD83}" name="data" displayName="data" ref="A1:G301" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A1:G301" xr:uid="{1EA555D6-243D-4A1C-9B7C-CE41EE1BDD83}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3AAD81AF-2B7E-4823-90E8-AEFBD60B475F}" name="Sales Person"/>
     <tableColumn id="2" xr3:uid="{6B2A071C-CA8E-4D5D-A456-93683388E25D}" name="Geography"/>
     <tableColumn id="3" xr3:uid="{71D03A3F-4D64-43CC-ACAF-CC0B5D52BBFA}" name="Product"/>
-    <tableColumn id="4" xr3:uid="{5D553C9D-CBC3-4141-A9EF-E2CCB295A7E8}" name="Amount" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{CE1F135C-B85B-45FB-A250-DD925A8AA3DC}" name="Units" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{DB0687AA-AACA-4EFC-A0A7-0E99C18CDE33}" name="Cost per unit" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{5D553C9D-CBC3-4141-A9EF-E2CCB295A7E8}" name="Amount" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{CE1F135C-B85B-45FB-A250-DD925A8AA3DC}" name="Units" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{DB0687AA-AACA-4EFC-A0A7-0E99C18CDE33}" name="Cost per unit" dataDxfId="21">
       <calculatedColumnFormula>_xlfn.XLOOKUP(data[[#This Row],[Product]],products[Product],products[Cost per unit])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DE9559EC-939B-4CD6-B200-FE941A0DF6C4}" name="Cost" dataDxfId="14">
+    <tableColumn id="7" xr3:uid="{DE9559EC-939B-4CD6-B200-FE941A0DF6C4}" name="Cost" dataDxfId="20">
       <calculatedColumnFormula>data[[#This Row],[Cost per unit]]*data[[#This Row],[Units]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8861,14 +8891,14 @@
   <autoFilter ref="I1:J23" xr:uid="{8063A97F-205E-4DAC-A81D-ECD217C80B46}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B2DE56DD-AD8A-4599-A5AF-F9AEFF673348}" name="Product"/>
-    <tableColumn id="2" xr3:uid="{6DF1EE73-09FF-4D82-AAC5-B07DFC203C2E}" name="Cost per unit" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{6DF1EE73-09FF-4D82-AAC5-B07DFC203C2E}" name="Cost per unit" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5161B1B2-F9B5-463A-A0B9-5EA20FB15509}" name="data4" displayName="data4" ref="A4:E304" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5161B1B2-F9B5-463A-A0B9-5EA20FB15509}" name="data4" displayName="data4" ref="A4:E304" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A4:E304" xr:uid="{5161B1B2-F9B5-463A-A0B9-5EA20FB15509}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:E304">
     <sortCondition descending="1" ref="D4:D304"/>
@@ -8877,22 +8907,22 @@
     <tableColumn id="1" xr3:uid="{7264495D-2BEA-4882-9EC2-9FBAAF61ECA5}" name="Sales Person"/>
     <tableColumn id="2" xr3:uid="{C993CC95-7731-4CFD-AA01-7D71D0E3B197}" name="Geography"/>
     <tableColumn id="3" xr3:uid="{B30DCE20-63A3-4649-A27D-7771A5D2CAE7}" name="Product"/>
-    <tableColumn id="4" xr3:uid="{7EC06B28-EE7E-4304-B3FE-C100CE159804}" name="Amount" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{202410D5-008A-42A0-A6B5-0BFF9151A388}" name="Units" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{7EC06B28-EE7E-4304-B3FE-C100CE159804}" name="Amount" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{202410D5-008A-42A0-A6B5-0BFF9151A388}" name="Units" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{53B737F6-EE5B-4D1A-BE39-7EB6DE09F1ED}" name="data5" displayName="data5" ref="M5:Q305" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{53B737F6-EE5B-4D1A-BE39-7EB6DE09F1ED}" name="data5" displayName="data5" ref="M5:Q305" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="M5:Q305" xr:uid="{53B737F6-EE5B-4D1A-BE39-7EB6DE09F1ED}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{E83CA7CB-B1C9-4834-9F12-3FFAC78D73D8}" name="Sales Person"/>
     <tableColumn id="2" xr3:uid="{E6106547-890B-431D-A830-408E3391D246}" name="Geography"/>
     <tableColumn id="3" xr3:uid="{B28AD51C-F80B-49CA-B423-FF2E73F79FEB}" name="Product"/>
-    <tableColumn id="4" xr3:uid="{0FA1E6B4-5852-43B0-853A-B11E18289F58}" name="Amount" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{727380C5-F872-40C9-9587-E9A5E85F8E98}" name="Units" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{0FA1E6B4-5852-43B0-853A-B11E18289F58}" name="Amount" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{727380C5-F872-40C9-9587-E9A5E85F8E98}" name="Units" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16779,10 +16809,10 @@
       <c r="A9" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9">
         <v>1197</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9">
         <v>573</v>
       </c>
       <c r="D9" s="32">
@@ -16799,10 +16829,10 @@
       <c r="A10" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10">
         <v>3612</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10">
         <v>384</v>
       </c>
       <c r="D10" s="32">
@@ -16819,10 +16849,10 @@
       <c r="A11" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11">
         <v>6132</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11">
         <v>93</v>
       </c>
       <c r="D11" s="32">
@@ -16836,10 +16866,10 @@
       <c r="A12" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12">
         <v>6391</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12">
         <v>48</v>
       </c>
       <c r="D12" s="32">
@@ -16856,10 +16886,10 @@
       <c r="A13" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13">
         <v>6391</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13">
         <v>738</v>
       </c>
       <c r="D13" s="32">
@@ -16876,10 +16906,10 @@
       <c r="A14" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14">
         <v>6398</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14">
         <v>102</v>
       </c>
       <c r="D14" s="32">
@@ -16893,10 +16923,10 @@
       <c r="A15" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="46">
+      <c r="B15">
         <v>7875</v>
       </c>
-      <c r="C15" s="46">
+      <c r="C15">
         <v>135</v>
       </c>
       <c r="D15" s="32">
@@ -16913,10 +16943,10 @@
       <c r="A16" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="46">
+      <c r="B16">
         <v>9702</v>
       </c>
-      <c r="C16" s="46">
+      <c r="C16">
         <v>243</v>
       </c>
       <c r="D16" s="32">
@@ -16930,10 +16960,10 @@
       <c r="A17" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="46">
+      <c r="B17">
         <v>10206</v>
       </c>
-      <c r="C17" s="46">
+      <c r="C17">
         <v>639</v>
       </c>
       <c r="D17" s="32">
@@ -16947,10 +16977,10 @@
       <c r="A18" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="46">
+      <c r="B18">
         <v>10661</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18">
         <v>219</v>
       </c>
       <c r="D18" s="32">
@@ -16964,10 +16994,10 @@
       <c r="A19" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="46">
+      <c r="B19">
         <v>12243</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19">
         <v>477</v>
       </c>
       <c r="D19" s="32">
@@ -16981,10 +17011,10 @@
       <c r="A20" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="46">
+      <c r="B20">
         <v>12369</v>
       </c>
-      <c r="C20" s="46">
+      <c r="C20">
         <v>312</v>
       </c>
       <c r="D20" s="32">
@@ -16998,10 +17028,10 @@
       <c r="A21" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="46">
+      <c r="B21">
         <v>12656</v>
       </c>
-      <c r="C21" s="46">
+      <c r="C21">
         <v>291</v>
       </c>
       <c r="D21" s="32">
@@ -17015,10 +17045,10 @@
       <c r="A22" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="46">
+      <c r="B22">
         <v>13076</v>
       </c>
-      <c r="C22" s="46">
+      <c r="C22">
         <v>240</v>
       </c>
       <c r="D22" s="32">
@@ -17032,10 +17062,10 @@
       <c r="A23" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="46">
+      <c r="B23">
         <v>13118</v>
       </c>
-      <c r="C23" s="46">
+      <c r="C23">
         <v>177</v>
       </c>
       <c r="D23" s="32">
@@ -17049,10 +17079,10 @@
       <c r="A24" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="46">
+      <c r="B24">
         <v>13286</v>
       </c>
-      <c r="C24" s="46">
+      <c r="C24">
         <v>303</v>
       </c>
       <c r="D24" s="32">
@@ -17066,10 +17096,10 @@
       <c r="A25" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="46">
+      <c r="B25">
         <v>14679</v>
       </c>
-      <c r="C25" s="46">
+      <c r="C25">
         <v>669</v>
       </c>
       <c r="D25" s="32">
@@ -17083,10 +17113,10 @@
       <c r="A26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="46">
+      <c r="B26">
         <v>16842</v>
       </c>
-      <c r="C26" s="46">
+      <c r="C26">
         <v>858</v>
       </c>
       <c r="D26" s="32">
@@ -17100,10 +17130,10 @@
       <c r="A27" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="46">
+      <c r="B27">
         <v>18396</v>
       </c>
-      <c r="C27" s="46">
+      <c r="C27">
         <v>456</v>
       </c>
       <c r="D27" s="32">
@@ -17117,10 +17147,10 @@
       <c r="A28" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="46">
+      <c r="B28">
         <v>23583</v>
       </c>
-      <c r="C28" s="46">
+      <c r="C28">
         <v>474</v>
       </c>
       <c r="D28" s="32">
@@ -17137,10 +17167,10 @@
       <c r="A29" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="46">
+      <c r="B29">
         <v>218813</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C29">
         <v>7431</v>
       </c>
       <c r="D29" s="32">
@@ -17181,7 +17211,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -30628,13 +30658,13 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -30723,10 +30753,10 @@
       <c r="B5" s="25">
         <v>252469</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="46">
         <v>252469</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="46">
         <v>8760</v>
       </c>
     </row>
@@ -30737,10 +30767,10 @@
       <c r="B6" s="25">
         <v>237944</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="46">
         <v>237944</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="46">
         <v>7302</v>
       </c>
     </row>
@@ -30751,10 +30781,10 @@
       <c r="B7" s="25">
         <v>218813</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="46">
         <v>218813</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="46">
         <v>7431</v>
       </c>
     </row>
@@ -30765,10 +30795,10 @@
       <c r="B8" s="25">
         <v>189434</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="46">
         <v>189434</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="46">
         <v>10158</v>
       </c>
     </row>
@@ -30779,10 +30809,10 @@
       <c r="B9" s="25">
         <v>173530</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="46">
         <v>173530</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="46">
         <v>5745</v>
       </c>
     </row>
@@ -30793,10 +30823,10 @@
       <c r="B10" s="25">
         <v>168679</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="46">
         <v>168679</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="46">
         <v>6264</v>
       </c>
     </row>

</xml_diff>